<commit_message>
convert carbon tax price to 2019 values, add guidance text
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB630F9-DD3C-4E70-8610-A7D0CE7CDA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381E7899-78CE-4569-96D6-0199AEC5083F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="435" windowWidth="14565" windowHeight="15810" activeTab="1" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="4350" yWindow="1605" windowWidth="22980" windowHeight="15000" activeTab="1" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="nonlignite_multiplier">#REF!</definedName>
     <definedName name="use_lifecycle_biofuel_EIs">[1]About!$A$61</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
   <si>
     <t>BCTR BAU Carbon Tax Rate</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t xml:space="preserve">As detailed on the "Projection" sheet, an exponential curve is fit to recent empirical data to project forward expected prices. </t>
+  </si>
+  <si>
+    <t>2019 to 2012 $</t>
   </si>
 </sst>
 </file>
@@ -2384,10 +2387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,6 +2513,14 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.89805481563188172</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2526,7 +2537,7 @@
   <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,132 +2651,132 @@
         <v>4</v>
       </c>
       <c r="B2" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C2" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D2" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E2" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F2" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G2" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H2" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I2" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J2" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K2" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L2" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M2" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N2" s="19">
         <f>$M$2</f>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O2" s="19">
         <f t="shared" ref="O2:AG9" si="0">$M$2</f>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG2" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -2773,132 +2784,132 @@
         <v>5</v>
       </c>
       <c r="B3" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C3" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D3" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E3" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F3" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G3" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H3" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I3" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J3" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K3" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L3" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M3" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N3" s="19">
         <f t="shared" ref="N3:AC9" si="1">$M$2</f>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC3" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD3" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE3" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF3" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG3" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -2906,132 +2917,132 @@
         <v>6</v>
       </c>
       <c r="B4" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C4" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D4" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E4" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F4" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G4" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H4" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I4" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J4" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K4" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L4" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M4" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N4" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG4" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -3039,132 +3050,132 @@
         <v>7</v>
       </c>
       <c r="B5" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C5" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D5" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E5" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F5" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G5" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H5" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I5" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J5" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K5" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L5" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M5" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N5" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG5" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -3172,132 +3183,132 @@
         <v>8</v>
       </c>
       <c r="B6" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C6" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D6" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E6" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F6" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G6" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H6" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I6" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J6" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K6" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L6" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M6" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N6" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG6" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
@@ -3305,398 +3316,398 @@
         <v>9</v>
       </c>
       <c r="B7" s="19">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
       </c>
       <c r="C7" s="19">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
       </c>
       <c r="D7" s="19">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
       </c>
       <c r="E7" s="19">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
       </c>
       <c r="F7" s="19">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
       </c>
       <c r="G7" s="19">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
       </c>
       <c r="H7" s="19">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
       </c>
       <c r="I7" s="19">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
       </c>
       <c r="J7" s="19">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
       </c>
       <c r="K7" s="19">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
       </c>
       <c r="L7" s="19">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
       </c>
       <c r="M7" s="19">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N7" s="19">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG7" s="19">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="8" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="20">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
-      </c>
-      <c r="C8" s="20">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
-      </c>
-      <c r="D8" s="20">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
-      </c>
-      <c r="E8" s="20">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
-      </c>
-      <c r="F8" s="20">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
-      </c>
-      <c r="G8" s="20">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
-      </c>
-      <c r="H8" s="20">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
-      </c>
-      <c r="I8" s="20">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
-      </c>
-      <c r="J8" s="20">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
-      </c>
-      <c r="K8" s="20">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
-      </c>
-      <c r="L8" s="20">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
-      </c>
-      <c r="M8" s="20">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+      <c r="B8" s="19">
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
+      </c>
+      <c r="C8" s="19">
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
+      </c>
+      <c r="D8" s="19">
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
+      </c>
+      <c r="E8" s="19">
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
+      </c>
+      <c r="F8" s="19">
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
+      </c>
+      <c r="G8" s="19">
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
+      </c>
+      <c r="H8" s="19">
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
+      </c>
+      <c r="I8" s="19">
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
+      </c>
+      <c r="J8" s="19">
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
+      </c>
+      <c r="K8" s="19">
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
+      </c>
+      <c r="L8" s="19">
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
+      </c>
+      <c r="M8" s="19">
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N8" s="20">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG8" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
     <row r="9" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20">
-        <f>Projection!$B$2</f>
-        <v>16.835000000000001</v>
-      </c>
-      <c r="C9" s="20">
-        <f>Projection!$C$2</f>
-        <v>17.227442207723623</v>
-      </c>
-      <c r="D9" s="20">
-        <f>Projection!D6</f>
-        <v>17.878404548930305</v>
-      </c>
-      <c r="E9" s="20">
-        <f>Projection!E6</f>
-        <v>19.010294056975361</v>
-      </c>
-      <c r="F9" s="20">
-        <f>Projection!F6</f>
-        <v>20.210676504452607</v>
-      </c>
-      <c r="G9" s="20">
-        <f>Projection!G6</f>
-        <v>21.483571461535131</v>
-      </c>
-      <c r="H9" s="20">
-        <f>Projection!H6</f>
-        <v>22.83322922306478</v>
-      </c>
-      <c r="I9" s="20">
-        <f>Projection!I6</f>
-        <v>24.264143832093552</v>
-      </c>
-      <c r="J9" s="20">
-        <f>Projection!J6</f>
-        <v>25.781066828967546</v>
-      </c>
-      <c r="K9" s="20">
-        <f>Projection!K6</f>
-        <v>27.389021765948701</v>
-      </c>
-      <c r="L9" s="20">
-        <f>Projection!L6</f>
-        <v>29.093319529555554</v>
-      </c>
-      <c r="M9" s="20">
-        <f>Projection!M6</f>
-        <v>30.89957451510822</v>
+      <c r="B9" s="19">
+        <f>Projection!B$2*About!$A$30</f>
+        <v>15.11875282116273</v>
+      </c>
+      <c r="C9" s="19">
+        <f>Projection!C$2*About!$A$30</f>
+        <v>15.471187435666137</v>
+      </c>
+      <c r="D9" s="19">
+        <f>Projection!D$2*About!$A$30</f>
+        <v>16.055787300981802</v>
+      </c>
+      <c r="E9" s="19">
+        <f>Projection!E$2*About!$A$30</f>
+        <v>17.072286124444865</v>
+      </c>
+      <c r="F9" s="19">
+        <f>Projection!F$2*About!$A$30</f>
+        <v>18.150295362001788</v>
+      </c>
+      <c r="G9" s="19">
+        <f>Projection!G$2*About!$A$30</f>
+        <v>19.293424808003287</v>
+      </c>
+      <c r="H9" s="19">
+        <f>Projection!H$2*About!$A$30</f>
+        <v>20.505491460199934</v>
+      </c>
+      <c r="I9" s="19">
+        <f>Projection!I$2*About!$A$30</f>
+        <v>21.790531215596236</v>
+      </c>
+      <c r="J9" s="19">
+        <f>Projection!J$2*About!$A$30</f>
+        <v>23.15281121788167</v>
+      </c>
+      <c r="K9" s="19">
+        <f>Projection!K$2*About!$A$30</f>
+        <v>24.596842892356655</v>
+      </c>
+      <c r="L9" s="19">
+        <f>Projection!L$2*About!$A$30</f>
+        <v>26.127395706234438</v>
+      </c>
+      <c r="M9" s="19">
+        <f>Projection!M$2*About!$A$30</f>
+        <v>27.749511694269103</v>
       </c>
       <c r="N9" s="20">
         <f t="shared" si="1"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="O9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="P9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Q9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="R9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="S9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="T9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="U9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="V9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="W9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="X9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Y9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="Z9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AA9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AB9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AC9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AD9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AE9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AF9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
       <c r="AG9" s="20">
         <f t="shared" si="0"/>
-        <v>30.89957451510822</v>
+        <v>27.749511694269103</v>
       </c>
     </row>
   </sheetData>
@@ -3710,7 +3721,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4270,7 +4281,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:XFD10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>